<commit_message>
New Program and Updates
</commit_message>
<xml_diff>
--- a/Docs/Program Templates v0.2.0.xlsx
+++ b/Docs/Program Templates v0.2.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/dennis_ad_unc_edu/Documents/Projects/Programs/Opentrons/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adminliveunc-my.sharepoint.com/personal/dennis_ad_unc_edu/Documents/Projects/Programs/Opentrons_Programs/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="499" documentId="8_{70C649BE-2B43-4933-89C5-D67F31D571D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A4F72E17-7D3D-4A93-98E5-65BAE7BE0F0F}"/>
+  <xr:revisionPtr revIDLastSave="540" documentId="8_{70C649BE-2B43-4933-89C5-D67F31D571D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{83724D38-884B-4CC4-9C21-5B632CF2E83C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="13455" yWindow="6390" windowWidth="7500" windowHeight="9210" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generic PCR" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="105">
   <si>
     <t>Source Well</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t># Illumina Indexing v0.1.0</t>
+  </si>
+  <si>
+    <t>Index Primers and Well Positions</t>
   </si>
 </sst>
 </file>
@@ -358,7 +361,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -452,8 +455,15 @@
       <sz val="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,8 +482,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -490,11 +506,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -543,6 +579,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -561,17 +603,42 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -735,6 +802,20 @@
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -749,31 +830,31 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E2D2C82-AED1-4EFD-B514-45C88869B632}" name="Table1" displayName="Table1" ref="A43:F451" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6E2D2C82-AED1-4EFD-B514-45C88869B632}" name="Table1" displayName="Table1" ref="A43:F451" totalsRowShown="0" headerRowDxfId="14">
   <autoFilter ref="A43:F451" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{869EDE9B-E883-4A3E-BC84-177627B77820}" name="# Source Slot"/>
     <tableColumn id="2" xr3:uid="{BFF29CE8-BC36-441D-BF7C-4D3ECA705071}" name="Source Well"/>
     <tableColumn id="3" xr3:uid="{BE3B5A50-56B7-458D-A1B8-EA325514A953}" name="Sample"/>
-    <tableColumn id="4" xr3:uid="{51C9CB7B-3C83-4DF7-B90E-3B3B2F0517EB}" name="Concentration ng/uL" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{F1CA2FD2-DD2B-44E5-934D-9BDE08DCFF66}" name="Destination Slot" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{7F589CB2-9FD4-4968-8CE1-91953E95F345}" name="Destination Well" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{51C9CB7B-3C83-4DF7-B90E-3B3B2F0517EB}" name="Concentration ng/uL" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{F1CA2FD2-DD2B-44E5-934D-9BDE08DCFF66}" name="Destination Slot" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{7F589CB2-9FD4-4968-8CE1-91953E95F345}" name="Destination Well" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A1EA636-4A66-4384-BAA4-76D238021771}" name="Table13" displayName="Table13" ref="A64:G472" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4A1EA636-4A66-4384-BAA4-76D238021771}" name="Table13" displayName="Table13" ref="A64:G472" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="A64:G472" xr:uid="{E9F71635-090B-4C48-B890-1CC5A8BA778F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{F86BB3DB-CF90-48B8-8F35-E42977442672}" name="# Source Slot"/>
     <tableColumn id="2" xr3:uid="{C0F53F8F-C6A8-4F67-BF04-2D1C3AE40DC7}" name="Source Well"/>
     <tableColumn id="8" xr3:uid="{466B28CD-7413-41AF-A6D9-1A9460F0F6F4}" name="Index"/>
     <tableColumn id="3" xr3:uid="{FB50DE30-1861-4AAD-B46A-522A9F77B092}" name="Sample"/>
-    <tableColumn id="4" xr3:uid="{624B6C14-EDFA-405E-9149-7A4DAA0A5782}" name="Concentration ng/uL" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{A82E5DDD-FDEB-4967-8780-CF48E4C9A4DF}" name="Destination Slot" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{28DE797A-4F93-44BF-AC9A-BA038C116648}" name="Destination Well" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{624B6C14-EDFA-405E-9149-7A4DAA0A5782}" name="Concentration ng/uL" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{A82E5DDD-FDEB-4967-8780-CF48E4C9A4DF}" name="Destination Slot" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{28DE797A-4F93-44BF-AC9A-BA038C116648}" name="Destination Well" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -979,8 +1060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B096AE39-CBE9-438B-8EF5-43BA511A3359}">
   <dimension ref="A1:I560"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1000,24 +1081,24 @@
         <v>63</v>
       </c>
       <c r="B1" s="5"/>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1040,123 +1121,123 @@
       <c r="A6" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
     </row>
     <row r="18" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
@@ -1214,24 +1295,24 @@
         <v>37</v>
       </c>
       <c r="B26" s="19"/>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
     </row>
     <row r="27" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="21"/>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
     </row>
     <row r="28" spans="1:6" ht="6.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
@@ -4116,12 +4197,12 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="D44:D451">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>($B$37/$D44)&gt;(0.5*$B$38)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3 B21:B22 B31:B33 B37:B39">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="15" priority="1">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4138,7 +4219,7 @@
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0B44E860-E070-40DD-B2DB-ECC1BE6D9400}">
           <x14:formula1>
             <xm:f>'Linked Values'!$A$3:$A$7</xm:f>
@@ -4149,13 +4230,7 @@
           <x14:formula1>
             <xm:f>'Linked Values'!$D$3:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>B22</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C4EB93F8-657F-47C1-B441-7EF353D4C600}">
-          <x14:formula1>
-            <xm:f>'Linked Values'!$D$3:$D$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>B21</xm:sqref>
+          <xm:sqref>B21:B22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4167,8 +4242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{547A22CE-6B5B-419C-B571-1556B7859EB9}">
   <dimension ref="A1:J581"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4230,135 +4305,135 @@
       <c r="A6" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="31"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="35"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
     </row>
     <row r="18" spans="1:7" ht="6.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13"/>
@@ -4369,14 +4444,14 @@
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
     </row>
-    <row r="19" spans="1:7" s="16" customFormat="1" ht="6.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" s="16" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="7"/>
+      <c r="B20" s="44"/>
       <c r="C20" s="7"/>
       <c r="D20" s="2"/>
     </row>
@@ -4420,24 +4495,24 @@
         <v>37</v>
       </c>
       <c r="B26" s="19"/>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
     </row>
     <row r="27" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="21"/>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" spans="1:7" ht="6.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13"/>
@@ -4455,9 +4530,11 @@
       <c r="D29" s="20"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="43" t="s">
         <v>23</v>
       </c>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
@@ -4494,203 +4571,205 @@
       <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35" s="42" t="s">
+        <v>104</v>
+      </c>
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="2"/>
+      <c r="C36" s="42"/>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="2"/>
+      <c r="C37" s="42"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="42"/>
       <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="2"/>
+      <c r="C39" s="42"/>
       <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="40" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="2"/>
+      <c r="C40" s="42"/>
       <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="40" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="2"/>
+      <c r="C41" s="42"/>
       <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="C42" s="2"/>
+      <c r="C42" s="42"/>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="6" t="s">
+      <c r="B43" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C43" s="2"/>
+      <c r="C43" s="42"/>
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="2"/>
+      <c r="C44" s="42"/>
       <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="C45" s="2"/>
+      <c r="C45" s="42"/>
       <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="6" t="s">
+      <c r="B46" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="2"/>
+      <c r="C46" s="42"/>
       <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="40" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="2"/>
+      <c r="C47" s="42"/>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="C48" s="2"/>
+      <c r="C48" s="42"/>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="2"/>
+      <c r="C49" s="42"/>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="2"/>
+      <c r="C50" s="42"/>
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="C51" s="2"/>
+      <c r="C51" s="42"/>
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="C52" s="2"/>
+      <c r="C52" s="42"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="2"/>
+      <c r="C53" s="42"/>
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="38" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="C54" s="2"/>
+      <c r="C54" s="42"/>
     </row>
     <row r="55" spans="1:10" ht="6.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="13"/>
@@ -4749,7 +4828,7 @@
       <c r="B64" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C64" s="36" t="s">
+      <c r="C64" s="30" t="s">
         <v>65</v>
       </c>
       <c r="D64" s="24" t="s">
@@ -7660,7 +7739,14 @@
       <c r="G581" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="15">
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="C35:C54"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A30:C30"/>
     <mergeCell ref="B16:G16"/>
     <mergeCell ref="B17:G17"/>
     <mergeCell ref="B10:G10"/>
@@ -7669,25 +7755,26 @@
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B9:G9"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <conditionalFormatting sqref="E65:E472">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>($B$58/$E65)&gt;(0.5*$B$59)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3 B21:B22 B31:B34">
-    <cfRule type="containsBlanks" dxfId="2" priority="2">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B58:B59">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(B58))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65:C472">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text=" ">
+      <formula>NOT(ISERROR(SEARCH(" ",C65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
@@ -7744,12 +7831,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="28" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">

</xml_diff>